<commit_message>
add import for marksize
</commit_message>
<xml_diff>
--- a/src/assets/documents/template-mark.xlsx
+++ b/src/assets/documents/template-mark.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WebstormProjects\expert-cable\frontend-public\src\assets\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F751BF03-D812-47B6-8174-964440456AD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CF4ECC1B-FA85-4AFC-8CDA-D6AD670E6016}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{780C6091-B73F-4F4F-AE82-DF9EEFDA6454}"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="2" r:id="rId1"/>
+    <sheet name="Импорт" sheetId="2" r:id="rId1"/>
+    <sheet name="Поля" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="101">
   <si>
     <t>Наименование марки</t>
   </si>
@@ -121,13 +122,229 @@
   </si>
   <si>
     <t>Центральный элемент</t>
+  </si>
+  <si>
+    <t>LAN кабели</t>
+  </si>
+  <si>
+    <t>Авиационные</t>
+  </si>
+  <si>
+    <t>Акустические</t>
+  </si>
+  <si>
+    <t>Антенные</t>
+  </si>
+  <si>
+    <t>Антивибрационные</t>
+  </si>
+  <si>
+    <t>Аудиокабели</t>
+  </si>
+  <si>
+    <t>Бортовые</t>
+  </si>
+  <si>
+    <t>Взрывные</t>
+  </si>
+  <si>
+    <t>Водопогружные</t>
+  </si>
+  <si>
+    <t>Высокочастотные</t>
+  </si>
+  <si>
+    <t>Геофизические</t>
+  </si>
+  <si>
+    <t>Грузонесущие</t>
+  </si>
+  <si>
+    <t>Для аэродромных огней</t>
+  </si>
+  <si>
+    <t>Для заземления</t>
+  </si>
+  <si>
+    <t>Для компьютерных сетей</t>
+  </si>
+  <si>
+    <t>Для медицинских приборов</t>
+  </si>
+  <si>
+    <t>Для подвижного состава</t>
+  </si>
+  <si>
+    <t>Для прогрева бетона</t>
+  </si>
+  <si>
+    <t>Для промышленной автоматизации и систем управления</t>
+  </si>
+  <si>
+    <t>Для систем пожарной и охранной сигнализации</t>
+  </si>
+  <si>
+    <t>Импортные</t>
+  </si>
+  <si>
+    <t>Импульсные</t>
+  </si>
+  <si>
+    <t>Интерфейсные</t>
+  </si>
+  <si>
+    <t>Коаксиальные</t>
+  </si>
+  <si>
+    <t>Контактные</t>
+  </si>
+  <si>
+    <t>Кроссовые</t>
+  </si>
+  <si>
+    <t>Ленточные</t>
+  </si>
+  <si>
+    <t>Магистральные</t>
+  </si>
+  <si>
+    <t>Металлические</t>
+  </si>
+  <si>
+    <t>Микрофонные</t>
+  </si>
+  <si>
+    <t>Нагревательные</t>
+  </si>
+  <si>
+    <t>Немагнитные</t>
+  </si>
+  <si>
+    <t>Нефтепогружные</t>
+  </si>
+  <si>
+    <t>Низкочастотные</t>
+  </si>
+  <si>
+    <t>Обмоточные</t>
+  </si>
+  <si>
+    <t>Оптические</t>
+  </si>
+  <si>
+    <t>Плавучие</t>
+  </si>
+  <si>
+    <t>Пневмокабель</t>
+  </si>
+  <si>
+    <t>Полевые</t>
+  </si>
+  <si>
+    <t>Проводного вещания</t>
+  </si>
+  <si>
+    <t>Радиотрансляционные</t>
+  </si>
+  <si>
+    <t>Радиочастотные</t>
+  </si>
+  <si>
+    <t>Резистивные</t>
+  </si>
+  <si>
+    <t>Релейные</t>
+  </si>
+  <si>
+    <t>Саморегулирующиеся</t>
+  </si>
+  <si>
+    <t>Сварочные</t>
+  </si>
+  <si>
+    <t>Связи</t>
+  </si>
+  <si>
+    <t>Сетевые</t>
+  </si>
+  <si>
+    <t>Сигнально-блокировочные</t>
+  </si>
+  <si>
+    <t>Сигнальные</t>
+  </si>
+  <si>
+    <t>Силовые</t>
+  </si>
+  <si>
+    <t>Силовые с резиновой изоляцией</t>
+  </si>
+  <si>
+    <t>Станционные</t>
+  </si>
+  <si>
+    <t>Судовые</t>
+  </si>
+  <si>
+    <t>Телефонные</t>
+  </si>
+  <si>
+    <t>Термопарные</t>
+  </si>
+  <si>
+    <t>Термостойкие</t>
+  </si>
+  <si>
+    <t>Термоэлектродные</t>
+  </si>
+  <si>
+    <t>Троллейбусные</t>
+  </si>
+  <si>
+    <t>Универсальные</t>
+  </si>
+  <si>
+    <t>Установочные</t>
+  </si>
+  <si>
+    <t>Холодостойкие</t>
+  </si>
+  <si>
+    <t>Шахтные</t>
+  </si>
+  <si>
+    <t>Экскаваторные</t>
+  </si>
+  <si>
+    <t>Электрические</t>
+  </si>
+  <si>
+    <t>Не бронированный</t>
+  </si>
+  <si>
+    <t>Бронированный</t>
+  </si>
+  <si>
+    <t>Лента</t>
+  </si>
+  <si>
+    <t>Проволока</t>
+  </si>
+  <si>
+    <t>Оплетка</t>
+  </si>
+  <si>
+    <t>Без заполнения</t>
+  </si>
+  <si>
+    <t>С заполнением</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,16 +360,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -160,16 +391,46 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -484,10 +745,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{199B1176-F458-49FB-8613-BA3F3DF15ACD}">
-  <dimension ref="A1:AC1"/>
+  <dimension ref="A1:AC11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y2" sqref="A2:XFD11"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -495,97 +756,668 @@
     <col min="1" max="29" width="20.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:29" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AA1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AB1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AC1" s="2" t="s">
         <v>28</v>
       </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+      <c r="AC2" s="3"/>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="3"/>
+      <c r="AC3" s="3"/>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+      <c r="AC4" s="3"/>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="3"/>
+      <c r="AC5" s="3"/>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="3"/>
+      <c r="AC6" s="3"/>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{66389731-8C02-495C-89FA-CB9183CE87D0}">
+          <x14:formula1>
+            <xm:f>Поля!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:G6</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{71CC02C8-FB65-4D86-9E9E-4CBEC2CA7D50}">
+          <x14:formula1>
+            <xm:f>Поля!$B$2:$B$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>K2:K6</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{F3308EDA-2B62-4455-A412-2CF70666696D}">
+          <x14:formula1>
+            <xm:f>Поля!$C$2:$C$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>S2:S6</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{5B663D23-0994-4380-9425-E0A5E4A7131A}">
+          <x14:formula1>
+            <xm:f>Поля!$D$2:$D$66</xm:f>
+          </x14:formula1>
+          <xm:sqref>Z2:Z6</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBAFF777-291F-4C8C-B7E8-59678A7D4607}">
+  <sheetPr codeName="Worksheet____1"/>
+  <dimension ref="A1:D66"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" customWidth="1"/>
+    <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D22" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D25" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D26" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D30" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D31" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D32" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D33" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D34" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D35" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D36" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D37" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D38" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="39" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D39" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="40" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D40" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="41" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D41" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="42" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D42" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="43" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D43" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="44" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D44" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="45" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D45" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="46" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D46" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="47" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D47" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="48" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D48" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D49" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D50" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="51" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D51" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="52" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D52" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="53" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D53" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="54" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D54" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="55" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D55" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="56" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D56" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="57" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D57" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="58" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D58" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="59" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D59" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="60" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D60" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="61" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D61" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="62" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D62" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="63" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D63" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="64" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D64" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="65" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D65" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="66" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D66" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>